<commit_message>
Atualização de conteúdo Higher Order Functions
</commit_message>
<xml_diff>
--- a/SoftSkills/Diário de Autoconhecimento.xlsx
+++ b/SoftSkills/Diário de Autoconhecimento.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t xml:space="preserve">Diário de Autoconhecimento</t>
   </si>
@@ -71,6 +71,48 @@
   </si>
   <si>
     <t xml:space="preserve">Pedir pra ele chegar perto e conversar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia de projeto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiquei ansioso. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descobri quem era minha dupla e fui conversar com ele. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">90% do projeto entregue.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiquei feliz com a parceria. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falei com minha dupla que fizemos um ótimo trabalho. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fazer compras de mês.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiquei ansioso e de mal humor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aceitei que tinha que fazer e tirei o foco de atenção nas compras. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gerar boletos para pagar contas do mês.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiquei estressado. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parei de gerar os boletos e retornei ao processo algumas horas depois. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia de projeto novo e véspera de mentoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acordei mais cedo para estudar o conteúdo para o projeto e refinar o material para a mentoria do dia seguinte.</t>
   </si>
 </sst>
 </file>
@@ -352,10 +394,10 @@
   <dimension ref="A1:Z1005"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="38.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="38.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.21"/>
@@ -596,7 +638,9 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14"/>
+      <c r="A8" s="14" t="n">
+        <v>44526</v>
+      </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -624,7 +668,9 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14"/>
+      <c r="A9" s="14" t="n">
+        <v>44527</v>
+      </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -652,7 +698,9 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14"/>
+      <c r="A10" s="14" t="n">
+        <v>44528</v>
+      </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -680,7 +728,9 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14"/>
+      <c r="A11" s="14" t="n">
+        <v>44529</v>
+      </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -708,7 +758,9 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14"/>
+      <c r="A12" s="14" t="n">
+        <v>44530</v>
+      </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -736,7 +788,9 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14"/>
+      <c r="A13" s="14" t="n">
+        <v>44531</v>
+      </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -764,15 +818,25 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14"/>
+      <c r="A14" s="14" t="n">
+        <v>44532</v>
+      </c>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="D14" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
+      <c r="G14" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>19</v>
+      </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -792,15 +856,25 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14"/>
-      <c r="B15" s="11"/>
+      <c r="A15" s="14" t="n">
+        <v>44533</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
+      <c r="G15" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -819,16 +893,26 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14"/>
+    <row r="16" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="14" t="n">
+        <v>44534</v>
+      </c>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
+      <c r="E16" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="F16" s="11"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
+      <c r="G16" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>25</v>
+      </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -847,16 +931,26 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14"/>
+    <row r="17" customFormat="false" ht="66.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14" t="n">
+        <v>44535</v>
+      </c>
       <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
+      <c r="C17" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
+      <c r="G17" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>28</v>
+      </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -876,7 +970,9 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14"/>
+      <c r="A18" s="14" t="n">
+        <v>44536</v>
+      </c>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -904,7 +1000,9 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14"/>
+      <c r="A19" s="14" t="n">
+        <v>44537</v>
+      </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -931,16 +1029,26 @@
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14"/>
+    <row r="20" customFormat="false" ht="67.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14" t="n">
+        <v>44538</v>
+      </c>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
+      <c r="D20" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
+      <c r="G20" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>30</v>
+      </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>

</xml_diff>